<commit_message>
v1.3 time was changed
</commit_message>
<xml_diff>
--- a/wykres gantta.xlsx
+++ b/wykres gantta.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Kamienie milowe</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Łączny czas pracy</t>
+  </si>
+  <si>
+    <t>Duże problemy z poprawieniem błędów w poruszaniu się. Więcej w post mortem</t>
   </si>
 </sst>
 </file>
@@ -625,11 +628,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="47665664"/>
-        <c:axId val="42884416"/>
+        <c:axId val="43733504"/>
+        <c:axId val="43867456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47665664"/>
+        <c:axId val="43733504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,7 +642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42884416"/>
+        <c:crossAx val="43867456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -647,7 +650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42884416"/>
+        <c:axId val="43867456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +661,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47665664"/>
+        <c:crossAx val="43733504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -923,7 +926,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,11 +1163,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="86889472"/>
-        <c:axId val="134559936"/>
+        <c:axId val="43735552"/>
+        <c:axId val="54446912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86889472"/>
+        <c:axId val="43735552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1177,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134559936"/>
+        <c:crossAx val="54446912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134559936"/>
+        <c:axId val="54446912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1196,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86889472"/>
+        <c:crossAx val="43735552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1584,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1693,10 @@
         <v>165</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>